<commit_message>
files structure change, final remarks
</commit_message>
<xml_diff>
--- a/Data_28.04.2023.xlsx
+++ b/Data_28.04.2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\P_nekhaeva\polar_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5687607-F413-477A-B8D4-AF3C9AC89183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A52D67D-1F21-4431-A593-15C91957F611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{1ED4DC13-57DD-2A40-8BAA-AE2EC4738D2D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="1" xr2:uid="{1ED4DC13-57DD-2A40-8BAA-AE2EC4738D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="logger_data" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1218,17 +1227,17 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="7" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.796875" style="5"/>
-    <col min="6" max="6" width="23.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.8125" style="5"/>
+    <col min="6" max="6" width="23.1875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
         <v>89</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>7.9234366327826917</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1308,7 +1317,7 @@
         <v>8.6143586203244951</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1328,7 +1337,7 @@
         <v>8.8520327665178016</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>8.5696310187091722</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1377,7 @@
         <v>8.4626857424132993</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>8.4069110793898325</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>8.7999170632820611</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1428,7 +1437,7 @@
         <v>9.0897069127111099</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1448,7 +1457,7 @@
         <v>8.8520327665178016</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>9.5284694991618526</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>10.114159593670568</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -1508,7 +1517,7 @@
         <v>10.224224567801974</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>10.326063349408116</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>9.5966371269866766</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>9.3513972848180789</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>9.9841245710511721</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -1608,7 +1617,7 @@
         <v>9.9138123339964661</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>8.3138257173288768</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
@@ -1648,7 +1657,7 @@
         <v>7.3031524800692784</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>6.8452117007847866</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>6.5562650002908258</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1717,7 @@
         <v>6.4685116425356108</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>6.3489805065176022</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
@@ -1748,7 +1757,7 @@
         <v>6.6374099919579495</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="8" t="s">
         <v>5</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>6.4901566482118929</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="9" t="s">
         <v>5</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>5.8092364140317576</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="9" t="s">
         <v>5</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>6.0268466701264547</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="9" t="s">
         <v>5</v>
       </c>
@@ -1828,7 +1837,7 @@
         <v>6.072863715836875</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="9" t="s">
         <v>5</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>6.210922111177239</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="9" t="s">
         <v>5</v>
       </c>
@@ -1868,7 +1877,7 @@
         <v>5.9932095875523279</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="9" t="s">
         <v>5</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>6.1465603476515369</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1917,7 @@
         <v>6.1507786096882162</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="9" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>6.5105549086959806</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="9" t="s">
         <v>5</v>
       </c>
@@ -1948,7 +1957,7 @@
         <v>6.7512542409415204</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="9" t="s">
         <v>5</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>6.9887409735181016</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="9" t="s">
         <v>5</v>
       </c>
@@ -1988,7 +1997,7 @@
         <v>6.6599112013155022</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="9" t="s">
         <v>5</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>7.3092703875598026</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="9" t="s">
         <v>5</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>7.8109310057458856</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="9" t="s">
         <v>5</v>
       </c>
@@ -2048,7 +2057,7 @@
         <v>7.9604094902423554</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="9" t="s">
         <v>5</v>
       </c>
@@ -2068,7 +2077,7 @@
         <v>8.2068466480993312</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
         <v>5</v>
       </c>
@@ -2088,7 +2097,7 @@
         <v>8.1642157940066973</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="9" t="s">
         <v>5</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>7.6813498748069762</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45" s="9" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>7.1456398548680333</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="9" t="s">
         <v>5</v>
       </c>
@@ -2148,7 +2157,7 @@
         <v>6.7849164481936626</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A47" s="9" t="s">
         <v>5</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>6.7323033218118766</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A48" s="9" t="s">
         <v>5</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>6.5883281266190421</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A49" s="9" t="s">
         <v>5</v>
       </c>
@@ -2208,7 +2217,7 @@
         <v>7.0631189869810012</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A50" s="9" t="s">
         <v>5</v>
       </c>
@@ -2228,7 +2237,7 @@
         <v>7.2470618085545748</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A51" s="10" t="s">
         <v>6</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>7.4563942966830279</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A52" s="6" t="s">
         <v>8</v>
       </c>
@@ -2268,7 +2277,7 @@
         <v>8.1911070411367426</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A53" s="6" t="s">
         <v>8</v>
       </c>
@@ -2288,7 +2297,7 @@
         <v>8.2451402861722674</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A54" s="6" t="s">
         <v>8</v>
       </c>
@@ -2308,7 +2317,7 @@
         <v>8.5184604054367643</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A55" s="6" t="s">
         <v>8</v>
       </c>
@@ -2328,7 +2337,7 @@
         <v>8.4069110793898325</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A56" s="6" t="s">
         <v>8</v>
       </c>
@@ -2348,7 +2357,7 @@
         <v>8.6300097314836961</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A57" s="6" t="s">
         <v>8</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>8.2991735312077957</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A58" s="6" t="s">
         <v>8</v>
       </c>
@@ -2388,7 +2397,7 @@
         <v>8.4069110793898325</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A59" s="6" t="s">
         <v>8</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>8.5120572326415758</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A60" s="6" t="s">
         <v>8</v>
       </c>
@@ -2428,7 +2437,7 @@
         <v>8.6194927353284321</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A61" s="6" t="s">
         <v>8</v>
       </c>
@@ -2448,7 +2457,7 @@
         <v>8.366381425311797</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A62" s="6" t="s">
         <v>8</v>
       </c>
@@ -2468,7 +2477,7 @@
         <v>8.8649725695162491</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A63" s="6" t="s">
         <v>8</v>
       </c>
@@ -2488,7 +2497,7 @@
         <v>8.8649725695162491</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A64" s="6" t="s">
         <v>8</v>
       </c>
@@ -2508,7 +2517,7 @@
         <v>9.6772152164386451</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A65" s="6" t="s">
         <v>8</v>
       </c>
@@ -2528,7 +2537,7 @@
         <v>9.9841245710511721</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A66" s="6" t="s">
         <v>8</v>
       </c>
@@ -2548,7 +2557,7 @@
         <v>9.7979045777614733</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A67" s="6" t="s">
         <v>8</v>
       </c>
@@ -2568,7 +2577,7 @@
         <v>9.5686601478908049</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A68" s="6" t="s">
         <v>8</v>
       </c>
@@ -2588,7 +2597,7 @@
         <v>9.3267438066211259</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A69" s="6" t="s">
         <v>8</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>8.8574908493496576</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A70" s="6" t="s">
         <v>8</v>
       </c>
@@ -2628,7 +2637,7 @@
         <v>8.6300097314836961</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A71" s="6" t="s">
         <v>8</v>
       </c>
@@ -2648,7 +2657,7 @@
         <v>8.5742350684602293</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A72" s="6" t="s">
         <v>8</v>
       </c>
@@ -2668,7 +2677,7 @@
         <v>8.6300097314836961</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A73" s="6" t="s">
         <v>8</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>8.5152894392345644</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A74" s="6" t="s">
         <v>8</v>
       </c>
@@ -2708,7 +2717,7 @@
         <v>8.1367310824831662</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A75" s="6" t="s">
         <v>8</v>
       </c>
@@ -2728,7 +2737,7 @@
         <v>8.1367310824831662</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A76" s="8" t="s">
         <v>9</v>
       </c>
@@ -2748,7 +2757,7 @@
         <v>8.1890704038979507</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A77" s="9" t="s">
         <v>9</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>8.1367310824831662</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A78" s="9" t="s">
         <v>9</v>
       </c>
@@ -2788,7 +2797,7 @@
         <v>8.1367310824831662</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A79" s="9" t="s">
         <v>9</v>
       </c>
@@ -2808,7 +2817,7 @@
         <v>8.1890704038979507</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A80" s="9" t="s">
         <v>9</v>
       </c>
@@ -2828,7 +2837,7 @@
         <v>8.4612561941990379</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A81" s="9" t="s">
         <v>9</v>
       </c>
@@ -2848,7 +2857,7 @@
         <v>8.2414014594691754</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A82" s="9" t="s">
         <v>9</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>8.2414014594691754</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A83" s="9" t="s">
         <v>9</v>
       </c>
@@ -2888,7 +2897,7 @@
         <v>8.4612561941990379</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A84" s="9" t="s">
         <v>9</v>
       </c>
@@ -2908,7 +2917,7 @@
         <v>8.2414014594691754</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A85" s="9" t="s">
         <v>9</v>
       </c>
@@ -2928,7 +2937,7 @@
         <v>9.0302031078549483</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A86" s="9" t="s">
         <v>9</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>8.7973425345021052</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A87" s="9" t="s">
         <v>9</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>9.7305458081115681</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A88" s="9" t="s">
         <v>9</v>
       </c>
@@ -2988,7 +2997,7 @@
         <v>9.6705638972027046</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A89" s="9" t="s">
         <v>9</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>8.5870045994268018</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A90" s="9" t="s">
         <v>9</v>
       </c>
@@ -3028,7 +3037,7 @@
         <v>7.7097294537325158</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A91" s="9" t="s">
         <v>9</v>
       </c>
@@ -3048,7 +3057,7 @@
         <v>7.9220927145327602</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A92" s="9" t="s">
         <v>9</v>
       </c>
@@ -3068,7 +3077,7 @@
         <v>7.5956347787813687</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A93" s="9" t="s">
         <v>9</v>
       </c>
@@ -3088,7 +3097,7 @@
         <v>7.2454885373394395</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A94" s="9" t="s">
         <v>9</v>
       </c>
@@ -3108,7 +3117,7 @@
         <v>7.1303500649017426</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A95" s="9" t="s">
         <v>9</v>
       </c>
@@ -3128,7 +3137,7 @@
         <v>6.4685116425356108</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A96" s="9" t="s">
         <v>9</v>
       </c>
@@ -3148,7 +3157,7 @@
         <v>6.7846633357040051</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A97" s="9" t="s">
         <v>9</v>
       </c>
@@ -3168,7 +3177,7 @@
         <v>6.3189234440766198</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A98" s="9" t="s">
         <v>9</v>
       </c>
@@ -3188,7 +3197,7 @@
         <v>5.8677529076237285</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A99" s="9" t="s">
         <v>9</v>
       </c>
@@ -3208,7 +3217,7 @@
         <v>5.3444191890765458</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A100" s="6" t="s">
         <v>10</v>
       </c>
@@ -3237,18 +3246,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9223C0-724D-894D-900C-5EDE0F5D5EEE}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="16.69921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" style="1"/>
-    <col min="5" max="17" width="10.796875" style="1"/>
+    <col min="3" max="3" width="16.6875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1875" style="1"/>
+    <col min="5" max="17" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
@@ -3295,7 +3302,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3348,7 +3355,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
@@ -3405,7 +3412,7 @@
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
     </row>
-    <row r="4" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>13</v>
       </c>
@@ -3458,7 +3465,7 @@
         <v>8.7222507128628202</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
@@ -3511,7 +3518,7 @@
         <v>9.808989955312061</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
@@ -3564,7 +3571,7 @@
         <v>9.8344069332521009</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -3617,7 +3624,7 @@
         <v>7.7864534464940478</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
@@ -3670,7 +3677,7 @@
         <v>6.5002647579027748</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
@@ -3723,7 +3730,7 @@
         <v>6.1220051118768435</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -3776,7 +3783,7 @@
         <v>6.2024051129530609</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
@@ -3829,7 +3836,7 @@
         <v>6.8439463424061815</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" s="15" t="s">
         <v>14</v>
       </c>
@@ -3882,7 +3889,7 @@
         <v>7.8903346651308137</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -3935,7 +3942,7 @@
         <v>7.3016850587374496</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -3988,7 +3995,7 @@
         <v>7.0174413081299054</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -4041,7 +4048,7 @@
         <v>8.3983257087238599</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
         <v>15</v>
       </c>
@@ -4094,7 +4101,7 @@
         <v>8.4935288620102654</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" s="15" t="s">
         <v>15</v>
       </c>
@@ -4147,7 +4154,7 @@
         <v>8.8786069032222734</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
@@ -4200,7 +4207,7 @@
         <v>9.6709296639526432</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" s="15" t="s">
         <v>15</v>
       </c>
@@ -4253,7 +4260,7 @@
         <v>8.8036978374796799</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" s="15" t="s">
         <v>15</v>
       </c>
@@ -4306,7 +4313,7 @@
         <v>8.3215663479165087</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="15" t="s">
         <v>16</v>
       </c>
@@ -4359,7 +4366,7 @@
         <v>8.2225718333922551</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -4412,7 +4419,7 @@
         <v>8.3293433533611196</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>16</v>
       </c>
@@ -4465,7 +4472,7 @@
         <v>9.0940113614281</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>16</v>
       </c>
@@ -4518,7 +4525,7 @@
         <v>8.2970050887352294</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
         <v>16</v>
       </c>
@@ -4571,7 +4578,7 @@
         <v>7.0449296718524321</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>16</v>
       </c>
@@ -4641,49 +4648,49 @@
       <selection pane="bottomRight" activeCell="LA5" sqref="LA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="41.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.09765625" customWidth="1"/>
-    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.796875" style="29"/>
-    <col min="29" max="29" width="10.796875" style="24"/>
-    <col min="30" max="40" width="10.796875"/>
-    <col min="41" max="41" width="10.796875" style="29"/>
-    <col min="55" max="55" width="10.796875" style="24"/>
-    <col min="56" max="66" width="10.796875"/>
-    <col min="67" max="67" width="10.796875" style="29"/>
-    <col min="81" max="81" width="10.796875" style="24"/>
-    <col min="82" max="92" width="10.796875"/>
-    <col min="93" max="93" width="10.796875" style="29"/>
-    <col min="107" max="107" width="10.796875" style="24"/>
-    <col min="108" max="118" width="10.796875"/>
-    <col min="119" max="119" width="10.796875" style="29"/>
-    <col min="132" max="132" width="10.796875" style="24"/>
-    <col min="133" max="143" width="10.796875"/>
-    <col min="144" max="144" width="10.796875" style="29"/>
-    <col min="157" max="157" width="10.796875" style="29"/>
-    <col min="158" max="158" width="10.796875" style="24"/>
-    <col min="159" max="169" width="10.796875"/>
-    <col min="170" max="170" width="10.796875" style="29"/>
-    <col min="184" max="184" width="10.796875" style="24"/>
-    <col min="185" max="195" width="10.796875"/>
-    <col min="196" max="196" width="10.796875" style="29"/>
-    <col min="210" max="210" width="10.796875" style="24"/>
-    <col min="211" max="222" width="10.796875"/>
-    <col min="236" max="236" width="10.796875" style="24"/>
-    <col min="237" max="247" width="10.796875"/>
-    <col min="248" max="248" width="10.796875" style="29"/>
-    <col min="262" max="262" width="10.796875" style="24"/>
-    <col min="263" max="273" width="10.796875"/>
-    <col min="274" max="274" width="10.796875" style="29"/>
-    <col min="288" max="288" width="10.796875" style="24"/>
-    <col min="289" max="299" width="10.796875"/>
-    <col min="300" max="300" width="10.796875" style="29"/>
-    <col min="313" max="313" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.8125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.8125" style="29"/>
+    <col min="29" max="29" width="10.8125" style="24"/>
+    <col min="30" max="40" width="10.8125"/>
+    <col min="41" max="41" width="10.8125" style="29"/>
+    <col min="55" max="55" width="10.8125" style="24"/>
+    <col min="56" max="66" width="10.8125"/>
+    <col min="67" max="67" width="10.8125" style="29"/>
+    <col min="81" max="81" width="10.8125" style="24"/>
+    <col min="82" max="92" width="10.8125"/>
+    <col min="93" max="93" width="10.8125" style="29"/>
+    <col min="107" max="107" width="10.8125" style="24"/>
+    <col min="108" max="118" width="10.8125"/>
+    <col min="119" max="119" width="10.8125" style="29"/>
+    <col min="132" max="132" width="10.8125" style="24"/>
+    <col min="133" max="143" width="10.8125"/>
+    <col min="144" max="144" width="10.8125" style="29"/>
+    <col min="157" max="157" width="10.8125" style="29"/>
+    <col min="158" max="158" width="10.8125" style="24"/>
+    <col min="159" max="169" width="10.8125"/>
+    <col min="170" max="170" width="10.8125" style="29"/>
+    <col min="184" max="184" width="10.8125" style="24"/>
+    <col min="185" max="195" width="10.8125"/>
+    <col min="196" max="196" width="10.8125" style="29"/>
+    <col min="210" max="210" width="10.8125" style="24"/>
+    <col min="211" max="222" width="10.8125"/>
+    <col min="236" max="236" width="10.8125" style="24"/>
+    <col min="237" max="247" width="10.8125"/>
+    <col min="248" max="248" width="10.8125" style="29"/>
+    <col min="262" max="262" width="10.8125" style="24"/>
+    <col min="263" max="273" width="10.8125"/>
+    <col min="274" max="274" width="10.8125" style="29"/>
+    <col min="288" max="288" width="10.8125" style="24"/>
+    <col min="289" max="299" width="10.8125"/>
+    <col min="300" max="300" width="10.8125" style="29"/>
+    <col min="313" max="313" width="13.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:313" s="30" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:313" s="30" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="30" t="s">
         <v>40</v>
       </c>
@@ -5624,7 +5631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:313" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:313" s="25" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A2" s="25" t="s">
         <v>30</v>
       </c>
@@ -6562,7 +6569,7 @@
         <v>42599</v>
       </c>
     </row>
-    <row r="3" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7500,7 +7507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -8752,7 +8759,7 @@
         <v>13_17_24:00 (12 a.m.)</v>
       </c>
     </row>
-    <row r="5" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -9693,7 +9700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:313" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:313" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -10634,7 +10641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -11575,7 +11582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -12516,7 +12523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -13457,7 +13464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -14398,7 +14405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -15339,7 +15346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -16280,7 +16287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -17221,7 +17228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -18162,7 +18169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A15" s="49" t="s">
         <v>51</v>
       </c>
@@ -19103,7 +19110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -20044,7 +20051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -20985,7 +20992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -21926,7 +21933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -22867,7 +22874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:313" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:313" x14ac:dyDescent="0.5">
       <c r="A20" s="49" t="s">
         <v>56</v>
       </c>
@@ -23808,7 +23815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:313" s="36" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:313" s="36" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="36" t="s">
         <v>57</v>
       </c>
@@ -24749,7 +24756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A22" s="48" t="s">
         <v>58</v>
       </c>
@@ -25690,7 +25697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A23" s="39" t="s">
         <v>59</v>
       </c>
@@ -26631,7 +26638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="39" t="s">
         <v>60</v>
       </c>
@@ -27572,7 +27579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A25" s="47" t="s">
         <v>66</v>
       </c>
@@ -28513,7 +28520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A26" s="47" t="s">
         <v>61</v>
       </c>
@@ -29454,7 +29461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A27" s="47" t="s">
         <v>62</v>
       </c>
@@ -30395,7 +30402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:313" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A28" s="39" t="s">
         <v>63</v>
       </c>

</xml_diff>